<commit_message>
Add example with multiple overdue disesases to example dataset
Example dataset - one client per id
</commit_message>
<xml_diff>
--- a/input/rodent_dataset.xlsx
+++ b/input/rodent_dataset.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justina\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FF2C98D-40DB-4A54-82D2-BF5F82B8DE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="91">
   <si>
     <t>School Type</t>
   </si>
@@ -202,9 +208,6 @@
     <t>N4U2L1</t>
   </si>
   <si>
-    <t>Varicella,</t>
-  </si>
-  <si>
     <t>Measles,</t>
   </si>
   <si>
@@ -287,13 +290,16 @@
   </si>
   <si>
     <t>[2014 MAR 12: DTaP-IPV-Hib, rota-unspecified] [2014 MAY 14: Pneu-C-13] [2014 JUL 19: DTaP-IPV-Hib] [2014 SEP 21: MMR] [2014 NOV 25: Men-C-C] [2015 APR 17: Var] [2015 SEP 13: DTaP-IPV-Hib] [2024 MAY 05: Tdap-IPV]</t>
+  </si>
+  <si>
+    <t>Varicella, HPV, Hepatitis B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -356,13 +362,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -400,7 +414,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -434,6 +448,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -468,9 +483,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -643,14 +659,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.6328125" customWidth="1"/>
+    <col min="2" max="2" width="31.26953125" customWidth="1"/>
+    <col min="3" max="3" width="22.90625" customWidth="1"/>
+    <col min="13" max="13" width="24.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -706,7 +730,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -741,25 +765,25 @@
         <v>57</v>
       </c>
       <c r="M2" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="N2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -794,25 +818,25 @@
         <v>58</v>
       </c>
       <c r="M3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="R3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -850,25 +874,25 @@
         <v>59</v>
       </c>
       <c r="M4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -903,25 +927,25 @@
         <v>60</v>
       </c>
       <c r="M5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -959,564 +983,22 @@
         <v>61</v>
       </c>
       <c r="M6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7">
-        <v>12</v>
-      </c>
-      <c r="G7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" t="s">
-        <v>51</v>
-      </c>
-      <c r="K7" t="s">
-        <v>56</v>
-      </c>
-      <c r="L7" t="s">
-        <v>57</v>
-      </c>
-      <c r="M7" t="s">
-        <v>62</v>
-      </c>
-      <c r="N7" t="s">
-        <v>67</v>
-      </c>
-      <c r="O7" t="s">
-        <v>71</v>
-      </c>
-      <c r="P7" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>81</v>
-      </c>
-      <c r="R7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" t="s">
-        <v>45</v>
-      </c>
-      <c r="J8" t="s">
-        <v>52</v>
-      </c>
-      <c r="K8" t="s">
-        <v>56</v>
-      </c>
-      <c r="L8" t="s">
-        <v>58</v>
-      </c>
-      <c r="M8" t="s">
-        <v>63</v>
-      </c>
-      <c r="N8" t="s">
-        <v>68</v>
-      </c>
-      <c r="O8" t="s">
-        <v>72</v>
-      </c>
-      <c r="P8" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>82</v>
-      </c>
-      <c r="R8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9">
-        <v>13</v>
-      </c>
-      <c r="G9" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" t="s">
-        <v>46</v>
-      </c>
-      <c r="I9" t="s">
-        <v>49</v>
-      </c>
-      <c r="J9" t="s">
-        <v>53</v>
-      </c>
-      <c r="K9" t="s">
-        <v>56</v>
-      </c>
-      <c r="L9" t="s">
-        <v>59</v>
-      </c>
-      <c r="M9" t="s">
-        <v>64</v>
-      </c>
-      <c r="N9" t="s">
-        <v>69</v>
-      </c>
-      <c r="O9" t="s">
-        <v>73</v>
-      </c>
-      <c r="P9" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>83</v>
-      </c>
-      <c r="R9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10">
-        <v>12</v>
-      </c>
-      <c r="G10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" t="s">
-        <v>47</v>
-      </c>
-      <c r="J10" t="s">
-        <v>54</v>
-      </c>
-      <c r="K10" t="s">
-        <v>56</v>
-      </c>
-      <c r="L10" t="s">
-        <v>60</v>
-      </c>
-      <c r="M10" t="s">
-        <v>65</v>
-      </c>
-      <c r="N10" t="s">
-        <v>68</v>
-      </c>
-      <c r="O10" t="s">
-        <v>74</v>
-      </c>
-      <c r="P10" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>84</v>
-      </c>
-      <c r="R10" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11">
-        <v>11</v>
-      </c>
-      <c r="G11" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" t="s">
-        <v>48</v>
-      </c>
-      <c r="I11" t="s">
-        <v>50</v>
-      </c>
-      <c r="J11" t="s">
-        <v>55</v>
-      </c>
-      <c r="K11" t="s">
-        <v>56</v>
-      </c>
-      <c r="L11" t="s">
-        <v>61</v>
-      </c>
-      <c r="M11" t="s">
-        <v>66</v>
-      </c>
-      <c r="N11" t="s">
-        <v>70</v>
-      </c>
-      <c r="O11" t="s">
-        <v>75</v>
-      </c>
-      <c r="P11" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>85</v>
-      </c>
-      <c r="R11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12">
-        <v>12</v>
-      </c>
-      <c r="G12" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" t="s">
-        <v>44</v>
-      </c>
-      <c r="J12" t="s">
-        <v>51</v>
-      </c>
-      <c r="K12" t="s">
-        <v>56</v>
-      </c>
-      <c r="L12" t="s">
-        <v>57</v>
-      </c>
-      <c r="M12" t="s">
-        <v>62</v>
-      </c>
-      <c r="N12" t="s">
-        <v>67</v>
-      </c>
-      <c r="O12" t="s">
-        <v>71</v>
-      </c>
-      <c r="P12" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>81</v>
-      </c>
-      <c r="R12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13">
-        <v>11</v>
-      </c>
-      <c r="G13" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" t="s">
-        <v>45</v>
-      </c>
-      <c r="J13" t="s">
-        <v>52</v>
-      </c>
-      <c r="K13" t="s">
-        <v>56</v>
-      </c>
-      <c r="L13" t="s">
-        <v>58</v>
-      </c>
-      <c r="M13" t="s">
-        <v>63</v>
-      </c>
-      <c r="N13" t="s">
-        <v>68</v>
-      </c>
-      <c r="O13" t="s">
-        <v>72</v>
-      </c>
-      <c r="P13" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>82</v>
-      </c>
-      <c r="R13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14">
-        <v>13</v>
-      </c>
-      <c r="G14" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" t="s">
-        <v>46</v>
-      </c>
-      <c r="I14" t="s">
-        <v>49</v>
-      </c>
-      <c r="J14" t="s">
-        <v>53</v>
-      </c>
-      <c r="K14" t="s">
-        <v>56</v>
-      </c>
-      <c r="L14" t="s">
-        <v>59</v>
-      </c>
-      <c r="M14" t="s">
-        <v>64</v>
-      </c>
-      <c r="N14" t="s">
-        <v>69</v>
-      </c>
-      <c r="O14" t="s">
-        <v>73</v>
-      </c>
-      <c r="P14" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>83</v>
-      </c>
-      <c r="R14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15">
-        <v>12</v>
-      </c>
-      <c r="G15" t="s">
-        <v>42</v>
-      </c>
-      <c r="H15" t="s">
-        <v>47</v>
-      </c>
-      <c r="J15" t="s">
-        <v>54</v>
-      </c>
-      <c r="K15" t="s">
-        <v>56</v>
-      </c>
-      <c r="L15" t="s">
-        <v>60</v>
-      </c>
-      <c r="M15" t="s">
-        <v>65</v>
-      </c>
-      <c r="N15" t="s">
-        <v>68</v>
-      </c>
-      <c r="O15" t="s">
-        <v>74</v>
-      </c>
-      <c r="P15" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>84</v>
-      </c>
-      <c r="R15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16">
-        <v>11</v>
-      </c>
-      <c r="G16" t="s">
-        <v>43</v>
-      </c>
-      <c r="H16" t="s">
-        <v>48</v>
-      </c>
-      <c r="I16" t="s">
-        <v>50</v>
-      </c>
-      <c r="J16" t="s">
-        <v>55</v>
-      </c>
-      <c r="K16" t="s">
-        <v>56</v>
-      </c>
-      <c r="L16" t="s">
-        <v>61</v>
-      </c>
-      <c r="M16" t="s">
-        <v>66</v>
-      </c>
-      <c r="N16" t="s">
-        <v>70</v>
-      </c>
-      <c r="O16" t="s">
-        <v>75</v>
-      </c>
-      <c r="P16" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>85</v>
-      </c>
-      <c r="R16" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modify a client to have multiple overdue diseases for demo purposes
</commit_message>
<xml_diff>
--- a/input/rodent_dataset.xlsx
+++ b/input/rodent_dataset.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justina\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FF2C98D-40DB-4A54-82D2-BF5F82B8DE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="91">
   <si>
     <t>School Type</t>
   </si>
@@ -202,9 +208,6 @@
     <t>N4U2L1</t>
   </si>
   <si>
-    <t>Varicella,</t>
-  </si>
-  <si>
     <t>Measles,</t>
   </si>
   <si>
@@ -287,13 +290,16 @@
   </si>
   <si>
     <t>[2014 MAR 12: DTaP-IPV-Hib, rota-unspecified] [2014 MAY 14: Pneu-C-13] [2014 JUL 19: DTaP-IPV-Hib] [2014 SEP 21: MMR] [2014 NOV 25: Men-C-C] [2015 APR 17: Var] [2015 SEP 13: DTaP-IPV-Hib] [2024 MAY 05: Tdap-IPV]</t>
+  </si>
+  <si>
+    <t>Varicella, HPV, Hepatitis B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -356,13 +362,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -400,7 +414,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -434,6 +448,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -468,9 +483,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -643,14 +659,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.6328125" customWidth="1"/>
+    <col min="2" max="2" width="31.26953125" customWidth="1"/>
+    <col min="3" max="3" width="22.90625" customWidth="1"/>
+    <col min="13" max="13" width="24.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -706,7 +730,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -741,25 +765,25 @@
         <v>57</v>
       </c>
       <c r="M2" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="N2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -794,25 +818,25 @@
         <v>58</v>
       </c>
       <c r="M3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="R3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -850,25 +874,25 @@
         <v>59</v>
       </c>
       <c r="M4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -903,25 +927,25 @@
         <v>60</v>
       </c>
       <c r="M5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -959,564 +983,22 @@
         <v>61</v>
       </c>
       <c r="M6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7">
-        <v>12</v>
-      </c>
-      <c r="G7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" t="s">
-        <v>51</v>
-      </c>
-      <c r="K7" t="s">
-        <v>56</v>
-      </c>
-      <c r="L7" t="s">
-        <v>57</v>
-      </c>
-      <c r="M7" t="s">
-        <v>62</v>
-      </c>
-      <c r="N7" t="s">
-        <v>67</v>
-      </c>
-      <c r="O7" t="s">
-        <v>71</v>
-      </c>
-      <c r="P7" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>81</v>
-      </c>
-      <c r="R7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" t="s">
-        <v>45</v>
-      </c>
-      <c r="J8" t="s">
-        <v>52</v>
-      </c>
-      <c r="K8" t="s">
-        <v>56</v>
-      </c>
-      <c r="L8" t="s">
-        <v>58</v>
-      </c>
-      <c r="M8" t="s">
-        <v>63</v>
-      </c>
-      <c r="N8" t="s">
-        <v>68</v>
-      </c>
-      <c r="O8" t="s">
-        <v>72</v>
-      </c>
-      <c r="P8" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>82</v>
-      </c>
-      <c r="R8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9">
-        <v>13</v>
-      </c>
-      <c r="G9" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" t="s">
-        <v>46</v>
-      </c>
-      <c r="I9" t="s">
-        <v>49</v>
-      </c>
-      <c r="J9" t="s">
-        <v>53</v>
-      </c>
-      <c r="K9" t="s">
-        <v>56</v>
-      </c>
-      <c r="L9" t="s">
-        <v>59</v>
-      </c>
-      <c r="M9" t="s">
-        <v>64</v>
-      </c>
-      <c r="N9" t="s">
-        <v>69</v>
-      </c>
-      <c r="O9" t="s">
-        <v>73</v>
-      </c>
-      <c r="P9" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>83</v>
-      </c>
-      <c r="R9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10">
-        <v>12</v>
-      </c>
-      <c r="G10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" t="s">
-        <v>47</v>
-      </c>
-      <c r="J10" t="s">
-        <v>54</v>
-      </c>
-      <c r="K10" t="s">
-        <v>56</v>
-      </c>
-      <c r="L10" t="s">
-        <v>60</v>
-      </c>
-      <c r="M10" t="s">
-        <v>65</v>
-      </c>
-      <c r="N10" t="s">
-        <v>68</v>
-      </c>
-      <c r="O10" t="s">
-        <v>74</v>
-      </c>
-      <c r="P10" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>84</v>
-      </c>
-      <c r="R10" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11">
-        <v>11</v>
-      </c>
-      <c r="G11" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" t="s">
-        <v>48</v>
-      </c>
-      <c r="I11" t="s">
-        <v>50</v>
-      </c>
-      <c r="J11" t="s">
-        <v>55</v>
-      </c>
-      <c r="K11" t="s">
-        <v>56</v>
-      </c>
-      <c r="L11" t="s">
-        <v>61</v>
-      </c>
-      <c r="M11" t="s">
-        <v>66</v>
-      </c>
-      <c r="N11" t="s">
-        <v>70</v>
-      </c>
-      <c r="O11" t="s">
-        <v>75</v>
-      </c>
-      <c r="P11" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>85</v>
-      </c>
-      <c r="R11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12">
-        <v>12</v>
-      </c>
-      <c r="G12" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" t="s">
-        <v>44</v>
-      </c>
-      <c r="J12" t="s">
-        <v>51</v>
-      </c>
-      <c r="K12" t="s">
-        <v>56</v>
-      </c>
-      <c r="L12" t="s">
-        <v>57</v>
-      </c>
-      <c r="M12" t="s">
-        <v>62</v>
-      </c>
-      <c r="N12" t="s">
-        <v>67</v>
-      </c>
-      <c r="O12" t="s">
-        <v>71</v>
-      </c>
-      <c r="P12" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>81</v>
-      </c>
-      <c r="R12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13">
-        <v>11</v>
-      </c>
-      <c r="G13" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" t="s">
-        <v>45</v>
-      </c>
-      <c r="J13" t="s">
-        <v>52</v>
-      </c>
-      <c r="K13" t="s">
-        <v>56</v>
-      </c>
-      <c r="L13" t="s">
-        <v>58</v>
-      </c>
-      <c r="M13" t="s">
-        <v>63</v>
-      </c>
-      <c r="N13" t="s">
-        <v>68</v>
-      </c>
-      <c r="O13" t="s">
-        <v>72</v>
-      </c>
-      <c r="P13" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>82</v>
-      </c>
-      <c r="R13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14">
-        <v>13</v>
-      </c>
-      <c r="G14" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" t="s">
-        <v>46</v>
-      </c>
-      <c r="I14" t="s">
-        <v>49</v>
-      </c>
-      <c r="J14" t="s">
-        <v>53</v>
-      </c>
-      <c r="K14" t="s">
-        <v>56</v>
-      </c>
-      <c r="L14" t="s">
-        <v>59</v>
-      </c>
-      <c r="M14" t="s">
-        <v>64</v>
-      </c>
-      <c r="N14" t="s">
-        <v>69</v>
-      </c>
-      <c r="O14" t="s">
-        <v>73</v>
-      </c>
-      <c r="P14" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>83</v>
-      </c>
-      <c r="R14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15">
-        <v>12</v>
-      </c>
-      <c r="G15" t="s">
-        <v>42</v>
-      </c>
-      <c r="H15" t="s">
-        <v>47</v>
-      </c>
-      <c r="J15" t="s">
-        <v>54</v>
-      </c>
-      <c r="K15" t="s">
-        <v>56</v>
-      </c>
-      <c r="L15" t="s">
-        <v>60</v>
-      </c>
-      <c r="M15" t="s">
-        <v>65</v>
-      </c>
-      <c r="N15" t="s">
-        <v>68</v>
-      </c>
-      <c r="O15" t="s">
-        <v>74</v>
-      </c>
-      <c r="P15" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>84</v>
-      </c>
-      <c r="R15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16">
-        <v>11</v>
-      </c>
-      <c r="G16" t="s">
-        <v>43</v>
-      </c>
-      <c r="H16" t="s">
-        <v>48</v>
-      </c>
-      <c r="I16" t="s">
-        <v>50</v>
-      </c>
-      <c r="J16" t="s">
-        <v>55</v>
-      </c>
-      <c r="K16" t="s">
-        <v>56</v>
-      </c>
-      <c r="L16" t="s">
-        <v>61</v>
-      </c>
-      <c r="M16" t="s">
-        <v>66</v>
-      </c>
-      <c r="N16" t="s">
-        <v>70</v>
-      </c>
-      <c r="O16" t="s">
-        <v>75</v>
-      </c>
-      <c r="P16" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>85</v>
-      </c>
-      <c r="R16" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjusted pytest to point to scripts for pythonpath in pytest.ini and work with test_cleanup.py; changed PyPDF2 to pypdf (PyPDF2 deprecated)
</commit_message>
<xml_diff>
--- a/input/rodent_dataset.xlsx
+++ b/input/rodent_dataset.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiat\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F584432-A7FB-4B22-BF66-40C9580D210A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="91">
   <si>
     <t>School Type</t>
   </si>
@@ -292,8 +298,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -356,13 +362,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -400,7 +414,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -434,6 +448,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -468,9 +483,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -643,14 +659,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14:R14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -706,7 +727,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -759,7 +780,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -812,7 +833,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -868,7 +889,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -921,7 +942,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -977,18 +998,18 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
-        <v>24</v>
+      <c r="C7">
+        <v>1009876548</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
         <v>34</v>
@@ -1012,33 +1033,33 @@
         <v>57</v>
       </c>
       <c r="M7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="O7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="P7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="Q7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="R7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
-        <v>25</v>
+      <c r="C8">
+        <v>1009876549</v>
       </c>
       <c r="D8" t="s">
         <v>30</v>
@@ -1065,33 +1086,33 @@
         <v>58</v>
       </c>
       <c r="M8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="R8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
-        <v>26</v>
+      <c r="C9">
+        <v>1009876550</v>
       </c>
       <c r="D9" t="s">
         <v>31</v>
@@ -1139,18 +1160,18 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" t="s">
-        <v>27</v>
+      <c r="C10">
+        <v>1009876551</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
         <v>37</v>
@@ -1192,18 +1213,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
       </c>
-      <c r="C11" t="s">
-        <v>28</v>
+      <c r="C11">
+        <v>1009876552</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
         <v>38</v>
@@ -1248,18 +1269,18 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>18</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="C12" t="s">
-        <v>24</v>
+      <c r="C12">
+        <v>1009876553</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
         <v>34</v>
@@ -1283,33 +1304,33 @@
         <v>57</v>
       </c>
       <c r="M12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="P12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="Q12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="R12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
       </c>
-      <c r="C13" t="s">
-        <v>25</v>
+      <c r="C13">
+        <v>1009876554</v>
       </c>
       <c r="D13" t="s">
         <v>30</v>
@@ -1354,15 +1375,15 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>18</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
       </c>
-      <c r="C14" t="s">
-        <v>26</v>
+      <c r="C14">
+        <v>1009876555</v>
       </c>
       <c r="D14" t="s">
         <v>31</v>
@@ -1392,33 +1413,33 @@
         <v>59</v>
       </c>
       <c r="M14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="P14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Q14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="R14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="B15" t="s">
         <v>22</v>
       </c>
-      <c r="C15" t="s">
-        <v>27</v>
+      <c r="C15">
+        <v>1009876556</v>
       </c>
       <c r="D15" t="s">
         <v>32</v>
@@ -1463,15 +1484,15 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>18</v>
       </c>
       <c r="B16" t="s">
         <v>23</v>
       </c>
-      <c r="C16" t="s">
-        <v>28</v>
+      <c r="C16">
+        <v>1009876557</v>
       </c>
       <c r="D16" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Adding row with incomplete address to the testing dataset for #115
</commit_message>
<xml_diff>
--- a/input/rodent_dataset.xlsx
+++ b/input/rodent_dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justina\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kassyr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FF2C98D-40DB-4A54-82D2-BF5F82B8DE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E213A50D-0CC0-4015-9BF3-34C3FE443494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-220" yWindow="580" windowWidth="18310" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="92">
   <si>
     <t>School Type</t>
   </si>
@@ -293,6 +293,9 @@
   </si>
   <si>
     <t>Varicella, HPV, Hepatitis B</t>
+  </si>
+  <si>
+    <t>Ratty</t>
   </si>
 </sst>
 </file>
@@ -351,11 +354,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -671,6 +675,7 @@
     <col min="1" max="1" width="21.6328125" customWidth="1"/>
     <col min="2" max="2" width="31.26953125" customWidth="1"/>
     <col min="3" max="3" width="22.90625" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24.81640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1001,6 +1006,56 @@
         <v>89</v>
       </c>
     </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7">
+        <v>1009876548</v>
+      </c>
+      <c r="D7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7">
+        <v>17</v>
+      </c>
+      <c r="G7" s="2">
+        <v>39872</v>
+      </c>
+      <c r="J7" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L7" t="s">
+        <v>61</v>
+      </c>
+      <c r="M7" t="s">
+        <v>65</v>
+      </c>
+      <c r="N7" t="s">
+        <v>69</v>
+      </c>
+      <c r="O7" t="s">
+        <v>74</v>
+      </c>
+      <c r="P7" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>84</v>
+      </c>
+      <c r="R7" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added example "Cheddarina Swiftpaws" to example dataset #79
</commit_message>
<xml_diff>
--- a/input/rodent_dataset.xlsx
+++ b/input/rodent_dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justina\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kassyr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FF2C98D-40DB-4A54-82D2-BF5F82B8DE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BDC915-33BF-4852-8C26-2DACB78E4916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="100">
   <si>
     <t>School Type</t>
   </si>
@@ -293,6 +293,33 @@
   </si>
   <si>
     <t>Varicella, HPV, Hepatitis B</t>
+  </si>
+  <si>
+    <t>Ratty</t>
+  </si>
+  <si>
+    <t>Cheddarina</t>
+  </si>
+  <si>
+    <t>Swiftpaws</t>
+  </si>
+  <si>
+    <t>44 Hayloft Road</t>
+  </si>
+  <si>
+    <t>H8Y6T6</t>
+  </si>
+  <si>
+    <t>MMR</t>
+  </si>
+  <si>
+    <t>TUNNEL ACADEMY-1009876550</t>
+  </si>
+  <si>
+    <t>Jan 10, 2015 - DTaP-IPV-Hib, Jan 29, 2015 - Pneu-C-13, Feb 18, 2015 - rota-unspecified, Mar 07, 2015 - DTaP-IPV-Hib, Mar 28, 2015 - MMR, Apr 15, 2015 - Men-C-C, May 02, 2015 - Var, May 27, 2015 - DTaP-IPV-Hib, Jun 16, 2015 - Pneu-C-13, Jul 09, 2015 - Influenza (IIV4), Aug 01, 2015 - Influenza (IIV4), Aug 29, 2015 - MMR, Sep 22, 2015 - Var, Oct 11, 2015 - DTaP-IPV-Hib, Nov 05, 2015 - Pneu-C-13, Dec 03, 2015 - Men-C-C, Jan 14, 2016 - MMR, Feb 06, 2016 - Influenza (IIV4), Mar 12, 2016 - Hep A, Apr 04, 2016 - Hep A booster, May 18, 2016 - Yellow Fever, Jun 07, 2016 - Rabies (pre-exposure), Jun 30, 2016 - Rabies (pre-exposure) dose 2, Jul 23, 2016 - Rabies (pre-exposure) dose 3, Aug 15, 2016 - Var, Sep 08, 2016 - DTaP-IPV-Hib, Oct 01, 2016 - Pneu-C-13, Oct 27, 2016 - Influenza (IIV4), Nov 19, 2016 - MMR, Dec 14, 2016 - Men-C-C, Jan 09, 2017 - Var, Feb 03, 2017 - DTaP-IPV-Hib, Mar 01, 2017 - Pneu-C-13, Mar 29, 2017 - MMR, Apr 18, 2017 - Influenza (IIV4), May 10, 2017 - COVID-19 (Pfizer Pediatric), Jun 02, 2017 - COVID-19 (Pfizer Pediatric) dose 2, Jun 28, 2017 - COVID-19 Booster, Jul 20, 2017 - Var, Aug 12, 2017 - Men-C-C, Sep 03, 2017 - Influenza (IIV4), Oct 25, 2017 - DTaP-IPV-Hib, Nov 16, 2017 - Pneu-C-13, Dec 08, 2017 - MMR, May 02, 2023 - Tdap, Jan 18, 2024 - Men-C-ACYW-135, May 01, 2024 - Tdap-IPV</t>
+  </si>
+  <si>
+    <t>[2015 JAN 10: DTaP-IPV-Hib] [2015 JAN 29: Pneu-C-13] [2015 FEB 18: rota-unspecified] [2015 MAR 07: DTaP-IPV-Hib] [2015 MAR 28: MMR] [2015 APR 15: Men-C-C] [2015 MAY 02: Var] [2015 MAY 27: DTaP-IPV-Hib] [2015 JUN 16: Pneu-C-13] [2015 JUL 09: Influenza (IIV4)] [2015 AUG 01: Influenza (IIV4)] [2015 AUG 29: MMR] [2015 SEP 22: Var] [2015 OCT 11: DTaP-IPV-Hib] [2015 NOV 05: Pneu-C-13] [2015 DEC 03: Men-C-C] [2016 JAN 14: MMR] [2016 FEB 06: Influenza (IIV4)] [2016 MAR 12: Hep A] [2016 APR 04: Hep A booster] [2016 MAY 18: Yellow Fever] [2016 JUN 07: Rabies (pre-exposure)] [2016 JUN 30: Rabies (pre-exposure) dose 2] [2016 JUL 23: Rabies (pre-exposure) dose 3] [2016 AUG 15: Var] [2016 SEP 08: DTaP-IPV-Hib] [2016 OCT 01: Pneu-C-13] [2016 OCT 27: Influenza (IIV4)] [2016 NOV 19: MMR] [2016 DEC 14: Men-C-C] [2017 JAN 09: Var] [2017 FEB 03: DTaP-IPV-Hib] [2017 MAR 01: Pneu-C-13] [2017 MAR 29: MMR] [2017 APR 18: Influenza (IIV4)] [2017 MAY 10: COVID-19 (Pfizer Pediatric)] [2017 JUN 02: COVID-19 (Pfizer Pediatric) dose 2] [2017 JUN 28: COVID-19 Booster] [2017 JUL 20: Var] [2017 AUG 12: Men-C-C] [2017 SEP 03: Influenza (IIV4)] [2017 OCT 25: DTaP-IPV-Hib] [2017 NOV 16: Pneu-C-13] [2017 DEC 08: MMR] [2023 MAY 02: Tdap] [2024 JAN 18: Men-C-ACYW-135] [2024 MAY 01: Tdap-IPV]</t>
   </si>
 </sst>
 </file>
@@ -351,11 +378,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A8" sqref="A8:R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -671,6 +699,7 @@
     <col min="1" max="1" width="21.6328125" customWidth="1"/>
     <col min="2" max="2" width="31.26953125" customWidth="1"/>
     <col min="3" max="3" width="22.90625" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24.81640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1001,6 +1030,109 @@
         <v>89</v>
       </c>
     </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7">
+        <v>1009876548</v>
+      </c>
+      <c r="D7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7">
+        <v>17</v>
+      </c>
+      <c r="G7" s="2">
+        <v>39872</v>
+      </c>
+      <c r="J7" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L7" t="s">
+        <v>61</v>
+      </c>
+      <c r="M7" t="s">
+        <v>65</v>
+      </c>
+      <c r="N7" t="s">
+        <v>69</v>
+      </c>
+      <c r="O7" t="s">
+        <v>74</v>
+      </c>
+      <c r="P7" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>84</v>
+      </c>
+      <c r="R7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8">
+        <v>1009876550</v>
+      </c>
+      <c r="D8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8">
+        <v>11</v>
+      </c>
+      <c r="G8" s="2">
+        <v>41896</v>
+      </c>
+      <c r="H8" t="s">
+        <v>94</v>
+      </c>
+      <c r="J8" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" t="s">
+        <v>95</v>
+      </c>
+      <c r="M8" t="s">
+        <v>96</v>
+      </c>
+      <c r="N8" t="s">
+        <v>96</v>
+      </c>
+      <c r="O8" t="s">
+        <v>98</v>
+      </c>
+      <c r="P8" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>81</v>
+      </c>
+      <c r="R8" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>